<commit_message>
changes on abastecedor file
</commit_message>
<xml_diff>
--- a/Datasets/Abastecedores_2025-10-01_2025-10-01.xlsx
+++ b/Datasets/Abastecedores_2025-10-01_2025-10-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofia\Documents\Data_Analytics_Ironhack\Projects\ironhack_final_project\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{EC01086D-E46E-4905-9D37-07AF6410FC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{14EEFA7F-F1F7-4720-A2B5-BA2ED84F3AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{2A4A056C-2E7C-40E0-AC2B-3807CB21F695}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="103">
   <si>
     <t>Produto</t>
   </si>
@@ -323,6 +323,12 @@
   </si>
   <si>
     <t>€/100kg</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Frutos</t>
   </si>
 </sst>
 </file>
@@ -1185,18 +1191,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E7F724C-C56C-4B06-869D-E8F6F1DD3E27}">
-  <dimension ref="A1:J65"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="6" max="6" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1204,31 +1210,34 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1236,32 +1245,35 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2">
-        <v>40</v>
-      </c>
-      <c r="F2" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G2" s="2">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>40</v>
+      </c>
+      <c r="G2" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H2" s="2">
         <v>2</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>2.5</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <v>2.4</v>
       </c>
-      <c r="J2">
-        <f>I2*100</f>
+      <c r="K2">
+        <f>J2*100</f>
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1269,32 +1281,35 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>40</v>
-      </c>
-      <c r="F3" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G3" s="2">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>40</v>
+      </c>
+      <c r="G3" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H3" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>2.7</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>2.5</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J65" si="0">I3*100</f>
+      <c r="K3">
+        <f t="shared" ref="K3:K65" si="0">J3*100</f>
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1302,32 +1317,35 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>40</v>
-      </c>
-      <c r="F4" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G4" s="2">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>40</v>
+      </c>
+      <c r="G4" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H4" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>1.8</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>1.2</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1335,32 +1353,35 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>40</v>
-      </c>
-      <c r="F5" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G5" s="2">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>40</v>
+      </c>
+      <c r="G5" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H5" s="2">
         <v>1</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>1.4</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <f t="shared" si="0"/>
         <v>110.00000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1368,32 +1389,35 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>40</v>
-      </c>
-      <c r="F6" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G6" s="2">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>40</v>
+      </c>
+      <c r="G6" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H6" s="2">
         <v>1.3</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>2</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>1.6</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <f t="shared" si="0"/>
         <v>160</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1401,32 +1425,35 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7">
-        <v>40</v>
-      </c>
-      <c r="F7" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G7" s="2">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>40</v>
+      </c>
+      <c r="G7" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H7" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>1.5</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>1.1499999999999999</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <f t="shared" si="0"/>
         <v>114.99999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1434,32 +1461,35 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8">
-        <v>40</v>
-      </c>
-      <c r="F8" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G8" s="2">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>40</v>
+      </c>
+      <c r="G8" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H8" s="2">
         <v>1.5</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>1.7</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>1.6</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <f t="shared" si="0"/>
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1467,32 +1497,35 @@
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9">
-        <v>40</v>
-      </c>
-      <c r="F9" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G9" s="2">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <v>40</v>
+      </c>
+      <c r="G9" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H9" s="2">
         <v>1</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <v>1.2</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>1.05</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -1500,32 +1533,35 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10">
-        <v>40</v>
-      </c>
-      <c r="F10" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G10" s="2">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>40</v>
+      </c>
+      <c r="G10" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H10" s="2">
         <v>2.1</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>2.15</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <f t="shared" si="0"/>
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1533,32 +1569,35 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11">
-        <v>40</v>
-      </c>
-      <c r="F11" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G11" s="2">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>40</v>
+      </c>
+      <c r="G11" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H11" s="2">
         <v>0.95</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <v>1</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1566,32 +1605,35 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12">
-        <v>40</v>
-      </c>
-      <c r="F12" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G12" s="2">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12">
+        <v>40</v>
+      </c>
+      <c r="G12" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H12" s="2">
         <v>0.95</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <v>1</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1599,32 +1641,35 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13">
-        <v>40</v>
-      </c>
-      <c r="F13" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G13" s="2">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>40</v>
+      </c>
+      <c r="G13" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H13" s="2">
         <v>0.95</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I13" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <v>1</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1632,32 +1677,35 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14">
-        <v>40</v>
-      </c>
-      <c r="F14" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G14" s="2">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>40</v>
+      </c>
+      <c r="G14" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H14" s="2">
         <v>2.0499999999999998</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>2.1</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <f t="shared" si="0"/>
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1665,32 +1713,35 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15">
-        <v>40</v>
-      </c>
-      <c r="F15" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G15" s="2">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15">
+        <v>40</v>
+      </c>
+      <c r="G15" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H15" s="2">
         <v>4</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>4.8</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>4.3</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <f t="shared" si="0"/>
         <v>430</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1698,32 +1749,35 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16">
-        <v>40</v>
-      </c>
-      <c r="F16" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G16" s="2">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16">
+        <v>40</v>
+      </c>
+      <c r="G16" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H16" s="2">
         <v>3.2</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>3.8</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <v>3.5</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1731,32 +1785,35 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17">
-        <v>40</v>
-      </c>
-      <c r="F17" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G17" s="2">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <v>40</v>
+      </c>
+      <c r="G17" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H17" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <v>1.8</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="2">
         <v>1.3</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1764,32 +1821,35 @@
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18">
-        <v>40</v>
-      </c>
-      <c r="F18" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G18" s="2">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18">
+        <v>40</v>
+      </c>
+      <c r="G18" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H18" s="2">
         <v>1.6</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I18" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J18" s="2">
         <v>1.8</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1797,32 +1857,35 @@
         <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19">
-        <v>40</v>
-      </c>
-      <c r="F19" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G19" s="2">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <v>40</v>
+      </c>
+      <c r="G19" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H19" s="2">
         <v>2</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I19" s="2">
         <v>2.8</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J19" s="2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <f t="shared" si="0"/>
         <v>229.99999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1830,32 +1893,35 @@
         <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20">
-        <v>40</v>
-      </c>
-      <c r="F20" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G20" s="2">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20">
+        <v>40</v>
+      </c>
+      <c r="G20" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H20" s="2">
         <v>2</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I20" s="2">
         <v>2.7</v>
       </c>
-      <c r="I20" s="2">
+      <c r="J20" s="2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <f t="shared" si="0"/>
         <v>229.99999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1863,32 +1929,35 @@
         <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21">
-        <v>40</v>
-      </c>
-      <c r="F21" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G21" s="2">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21">
+        <v>40</v>
+      </c>
+      <c r="G21" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H21" s="2">
         <v>3.5</v>
       </c>
-      <c r="H21" s="2">
+      <c r="I21" s="2">
         <v>4.2</v>
       </c>
-      <c r="I21" s="2">
+      <c r="J21" s="2">
         <v>4</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1896,32 +1965,35 @@
         <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22">
-        <v>40</v>
-      </c>
-      <c r="F22" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G22" s="2">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22">
+        <v>40</v>
+      </c>
+      <c r="G22" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H22" s="2">
         <v>2.8</v>
       </c>
-      <c r="H22" s="2">
+      <c r="I22" s="2">
         <v>3.5</v>
       </c>
-      <c r="I22" s="2">
+      <c r="J22" s="2">
         <v>3.3</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <f t="shared" si="0"/>
         <v>330</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1929,32 +2001,35 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23">
-        <v>40</v>
-      </c>
-      <c r="F23" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G23" s="2">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23">
+        <v>40</v>
+      </c>
+      <c r="G23" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H23" s="2">
         <v>1.3</v>
       </c>
-      <c r="H23" s="2">
+      <c r="I23" s="2">
         <v>1.7</v>
       </c>
-      <c r="I23" s="2">
+      <c r="J23" s="2">
         <v>1.6</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <f t="shared" si="0"/>
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1962,32 +2037,35 @@
         <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24">
-        <v>40</v>
-      </c>
-      <c r="F24" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G24" s="2">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24">
+        <v>40</v>
+      </c>
+      <c r="G24" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H24" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H24" s="2">
+      <c r="I24" s="2">
         <v>1.5</v>
       </c>
-      <c r="I24" s="2">
+      <c r="J24" s="2">
         <v>1.2</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -1995,32 +2073,35 @@
         <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25">
-        <v>40</v>
-      </c>
-      <c r="F25" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G25" s="2">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25">
+        <v>40</v>
+      </c>
+      <c r="G25" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H25" s="2">
         <v>2</v>
       </c>
-      <c r="H25" s="2">
+      <c r="I25" s="2">
         <v>2.5</v>
       </c>
-      <c r="I25" s="2">
+      <c r="J25" s="2">
         <v>2.1</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <f t="shared" si="0"/>
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -2028,32 +2109,35 @@
         <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26">
-        <v>40</v>
-      </c>
-      <c r="F26" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G26" s="2">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26">
+        <v>40</v>
+      </c>
+      <c r="G26" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H26" s="2">
         <v>1.6</v>
       </c>
-      <c r="H26" s="2">
+      <c r="I26" s="2">
         <v>2</v>
       </c>
-      <c r="I26" s="2">
+      <c r="J26" s="2">
         <v>1.8</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>49</v>
       </c>
@@ -2061,32 +2145,35 @@
         <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27">
-        <v>40</v>
-      </c>
-      <c r="F27" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G27" s="2">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27">
+        <v>40</v>
+      </c>
+      <c r="G27" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H27" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H27" s="2">
+      <c r="I27" s="2">
         <v>1.7</v>
       </c>
-      <c r="I27" s="2">
+      <c r="J27" s="2">
         <v>1.3</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -2094,32 +2181,35 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28">
-        <v>40</v>
-      </c>
-      <c r="F28" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G28" s="2">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28">
+        <v>40</v>
+      </c>
+      <c r="G28" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H28" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H28" s="2">
+      <c r="I28" s="2">
         <v>1.7</v>
       </c>
-      <c r="I28" s="2">
+      <c r="J28" s="2">
         <v>1.3</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -2127,32 +2217,35 @@
         <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29">
-        <v>40</v>
-      </c>
-      <c r="F29" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G29" s="2">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29">
+        <v>40</v>
+      </c>
+      <c r="G29" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H29" s="2">
         <v>1</v>
       </c>
-      <c r="H29" s="2">
+      <c r="I29" s="2">
         <v>1.2</v>
       </c>
-      <c r="I29" s="2">
+      <c r="J29" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <f t="shared" si="0"/>
         <v>110.00000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -2160,32 +2253,35 @@
         <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30">
-        <v>40</v>
-      </c>
-      <c r="F30" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G30" s="2">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30">
+        <v>40</v>
+      </c>
+      <c r="G30" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H30" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H30" s="2">
+      <c r="I30" s="2">
         <v>1.3</v>
       </c>
-      <c r="I30" s="2">
+      <c r="J30" s="2">
         <v>1.2</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -2193,32 +2289,35 @@
         <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31">
-        <v>40</v>
-      </c>
-      <c r="F31" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G31" s="2">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31">
+        <v>40</v>
+      </c>
+      <c r="G31" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H31" s="2">
         <v>1.2</v>
       </c>
-      <c r="H31" s="2">
+      <c r="I31" s="2">
         <v>1.45</v>
       </c>
-      <c r="I31" s="2">
+      <c r="J31" s="2">
         <v>1.3</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -2226,32 +2325,35 @@
         <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D32" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32">
-        <v>40</v>
-      </c>
-      <c r="F32" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G32" s="2">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32">
+        <v>40</v>
+      </c>
+      <c r="G32" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H32" s="2">
         <v>0.75</v>
       </c>
-      <c r="H32" s="2">
+      <c r="I32" s="2">
         <v>1</v>
       </c>
-      <c r="I32" s="2">
+      <c r="J32" s="2">
         <v>0.8</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>56</v>
       </c>
@@ -2259,32 +2361,35 @@
         <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
-      </c>
-      <c r="E33">
-        <v>40</v>
-      </c>
-      <c r="F33" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G33" s="2">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33">
+        <v>40</v>
+      </c>
+      <c r="G33" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H33" s="2">
         <v>0.8</v>
       </c>
-      <c r="H33" s="2">
+      <c r="I33" s="2">
         <v>1.05</v>
       </c>
-      <c r="I33" s="2">
+      <c r="J33" s="2">
         <v>0.85</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>57</v>
       </c>
@@ -2292,32 +2397,35 @@
         <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34">
-        <v>40</v>
-      </c>
-      <c r="F34" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G34" s="2">
+        <v>11</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34">
+        <v>40</v>
+      </c>
+      <c r="G34" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H34" s="2">
         <v>0.85</v>
       </c>
-      <c r="H34" s="2">
+      <c r="I34" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I34" s="2">
+      <c r="J34" s="2">
         <v>0.9</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -2325,32 +2433,35 @@
         <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D35" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35">
-        <v>40</v>
-      </c>
-      <c r="F35" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G35" s="2">
+        <v>11</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35">
+        <v>40</v>
+      </c>
+      <c r="G35" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H35" s="2">
         <v>0.85</v>
       </c>
-      <c r="H35" s="2">
+      <c r="I35" s="2">
         <v>1.05</v>
       </c>
-      <c r="I35" s="2">
+      <c r="J35" s="2">
         <v>0.95</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>59</v>
       </c>
@@ -2358,32 +2469,35 @@
         <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36">
-        <v>40</v>
-      </c>
-      <c r="F36" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G36" s="2">
+        <v>11</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36">
+        <v>40</v>
+      </c>
+      <c r="G36" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H36" s="2">
         <v>0.9</v>
       </c>
-      <c r="H36" s="2">
+      <c r="I36" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I36" s="2">
+      <c r="J36" s="2">
         <v>1</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>60</v>
       </c>
@@ -2391,32 +2505,35 @@
         <v>52</v>
       </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D37" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37">
-        <v>40</v>
-      </c>
-      <c r="F37" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G37" s="2">
+        <v>11</v>
+      </c>
+      <c r="E37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37">
+        <v>40</v>
+      </c>
+      <c r="G37" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H37" s="2">
         <v>0.75</v>
       </c>
-      <c r="H37" s="2">
+      <c r="I37" s="2">
         <v>0.9</v>
       </c>
-      <c r="I37" s="2">
+      <c r="J37" s="2">
         <v>0.85</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>61</v>
       </c>
@@ -2424,32 +2541,35 @@
         <v>52</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D38" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38">
-        <v>40</v>
-      </c>
-      <c r="F38" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G38" s="2">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38">
+        <v>40</v>
+      </c>
+      <c r="G38" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H38" s="2">
         <v>0.8</v>
       </c>
-      <c r="H38" s="2">
+      <c r="I38" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="I38" s="2">
+      <c r="J38" s="2">
         <v>0.95</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>62</v>
       </c>
@@ -2457,32 +2577,35 @@
         <v>52</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D39" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39">
-        <v>40</v>
-      </c>
-      <c r="F39" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G39" s="2">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39">
+        <v>40</v>
+      </c>
+      <c r="G39" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H39" s="2">
         <v>0.7</v>
       </c>
-      <c r="H39" s="2">
+      <c r="I39" s="2">
         <v>0.9</v>
       </c>
-      <c r="I39" s="2">
+      <c r="J39" s="2">
         <v>0.8</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -2490,32 +2613,35 @@
         <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D40" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40">
-        <v>40</v>
-      </c>
-      <c r="F40" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G40" s="2">
+        <v>11</v>
+      </c>
+      <c r="E40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40">
+        <v>40</v>
+      </c>
+      <c r="G40" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H40" s="2">
         <v>3</v>
       </c>
-      <c r="H40" s="2">
+      <c r="I40" s="2">
         <v>3.5</v>
       </c>
-      <c r="I40" s="2">
+      <c r="J40" s="2">
         <v>3.2</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <f t="shared" si="0"/>
         <v>320</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>65</v>
       </c>
@@ -2523,32 +2649,35 @@
         <v>64</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D41" t="s">
-        <v>12</v>
-      </c>
-      <c r="E41">
-        <v>40</v>
-      </c>
-      <c r="F41" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G41" s="2">
+        <v>11</v>
+      </c>
+      <c r="E41" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41">
+        <v>40</v>
+      </c>
+      <c r="G41" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H41" s="2">
         <v>1.4</v>
       </c>
-      <c r="H41" s="2">
+      <c r="I41" s="2">
         <v>1.8</v>
       </c>
-      <c r="I41" s="2">
+      <c r="J41" s="2">
         <v>1.5</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>66</v>
       </c>
@@ -2556,32 +2685,35 @@
         <v>64</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D42" t="s">
-        <v>12</v>
-      </c>
-      <c r="E42">
-        <v>40</v>
-      </c>
-      <c r="F42" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G42" s="2">
+        <v>11</v>
+      </c>
+      <c r="E42" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42">
+        <v>40</v>
+      </c>
+      <c r="G42" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H42" s="2">
         <v>1.5</v>
       </c>
-      <c r="H42" s="2">
+      <c r="I42" s="2">
         <v>1.9</v>
       </c>
-      <c r="I42" s="2">
+      <c r="J42" s="2">
         <v>1.7</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <f t="shared" si="0"/>
         <v>170</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>67</v>
       </c>
@@ -2589,32 +2721,35 @@
         <v>68</v>
       </c>
       <c r="C43" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D43" t="s">
-        <v>12</v>
-      </c>
-      <c r="E43">
-        <v>40</v>
-      </c>
-      <c r="F43" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G43" s="2">
+        <v>11</v>
+      </c>
+      <c r="E43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43">
+        <v>40</v>
+      </c>
+      <c r="G43" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H43" s="2">
         <v>0.25</v>
       </c>
-      <c r="H43" s="2">
+      <c r="I43" s="2">
         <v>0.45</v>
       </c>
-      <c r="I43" s="2">
+      <c r="J43" s="2">
         <v>0.3</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -2622,32 +2757,35 @@
         <v>68</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D44" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44">
-        <v>40</v>
-      </c>
-      <c r="F44" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G44" s="2">
+        <v>11</v>
+      </c>
+      <c r="E44" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44">
+        <v>40</v>
+      </c>
+      <c r="G44" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H44" s="2">
         <v>0.25</v>
       </c>
-      <c r="H44" s="2">
+      <c r="I44" s="2">
         <v>0.45</v>
       </c>
-      <c r="I44" s="2">
+      <c r="J44" s="2">
         <v>0.35</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -2655,32 +2793,35 @@
         <v>68</v>
       </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D45" t="s">
-        <v>12</v>
-      </c>
-      <c r="E45">
-        <v>40</v>
-      </c>
-      <c r="F45" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G45" s="2">
+        <v>11</v>
+      </c>
+      <c r="E45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45">
+        <v>40</v>
+      </c>
+      <c r="G45" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H45" s="2">
         <v>0.25</v>
       </c>
-      <c r="H45" s="2">
+      <c r="I45" s="2">
         <v>0.45</v>
       </c>
-      <c r="I45" s="2">
+      <c r="J45" s="2">
         <v>0.3</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>71</v>
       </c>
@@ -2688,32 +2829,35 @@
         <v>68</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46">
-        <v>40</v>
-      </c>
-      <c r="F46" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G46" s="2">
+        <v>11</v>
+      </c>
+      <c r="E46" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46">
+        <v>40</v>
+      </c>
+      <c r="G46" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H46" s="2">
         <v>0.3</v>
       </c>
-      <c r="H46" s="2">
+      <c r="I46" s="2">
         <v>0.5</v>
       </c>
-      <c r="I46" s="2">
+      <c r="J46" s="2">
         <v>0.35</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>72</v>
       </c>
@@ -2721,32 +2865,35 @@
         <v>73</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D47" t="s">
-        <v>12</v>
-      </c>
-      <c r="E47">
-        <v>40</v>
-      </c>
-      <c r="F47" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G47" s="2">
+        <v>11</v>
+      </c>
+      <c r="E47" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47">
+        <v>40</v>
+      </c>
+      <c r="G47" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H47" s="2">
         <v>0.3</v>
       </c>
-      <c r="H47" s="2">
+      <c r="I47" s="2">
         <v>0.5</v>
       </c>
-      <c r="I47" s="2">
+      <c r="J47" s="2">
         <v>0.4</v>
       </c>
-      <c r="J47">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K47">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>74</v>
       </c>
@@ -2754,32 +2901,35 @@
         <v>73</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D48" t="s">
-        <v>12</v>
-      </c>
-      <c r="E48">
-        <v>40</v>
-      </c>
-      <c r="F48" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G48" s="2">
+        <v>11</v>
+      </c>
+      <c r="E48" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48">
+        <v>40</v>
+      </c>
+      <c r="G48" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H48" s="2">
         <v>0.3</v>
       </c>
-      <c r="H48" s="2">
+      <c r="I48" s="2">
         <v>0.5</v>
       </c>
-      <c r="I48" s="2">
+      <c r="J48" s="2">
         <v>0.35</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>75</v>
       </c>
@@ -2787,32 +2937,35 @@
         <v>73</v>
       </c>
       <c r="C49" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D49" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49">
-        <v>40</v>
-      </c>
-      <c r="F49" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G49" s="2">
+        <v>11</v>
+      </c>
+      <c r="E49" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49">
+        <v>40</v>
+      </c>
+      <c r="G49" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H49" s="2">
         <v>0.3</v>
       </c>
-      <c r="H49" s="2">
+      <c r="I49" s="2">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I49" s="2">
+      <c r="J49" s="2">
         <v>0.35</v>
       </c>
-      <c r="J49">
+      <c r="K49">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>76</v>
       </c>
@@ -2820,32 +2973,35 @@
         <v>73</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D50" t="s">
-        <v>12</v>
-      </c>
-      <c r="E50">
-        <v>40</v>
-      </c>
-      <c r="F50" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G50" s="2">
+        <v>11</v>
+      </c>
+      <c r="E50" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50">
+        <v>40</v>
+      </c>
+      <c r="G50" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H50" s="2">
         <v>0.3</v>
       </c>
-      <c r="H50" s="2">
+      <c r="I50" s="2">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I50" s="2">
+      <c r="J50" s="2">
         <v>0.4</v>
       </c>
-      <c r="J50">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K50">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>77</v>
       </c>
@@ -2853,32 +3009,35 @@
         <v>78</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D51" t="s">
-        <v>12</v>
-      </c>
-      <c r="E51">
-        <v>40</v>
-      </c>
-      <c r="F51" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G51" s="2">
+        <v>11</v>
+      </c>
+      <c r="E51" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51">
+        <v>40</v>
+      </c>
+      <c r="G51" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H51" s="2">
         <v>0.8</v>
       </c>
-      <c r="H51" s="2">
+      <c r="I51" s="2">
         <v>1.3</v>
       </c>
-      <c r="I51" s="2">
+      <c r="J51" s="2">
         <v>0.9</v>
       </c>
-      <c r="J51">
+      <c r="K51">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>79</v>
       </c>
@@ -2886,32 +3045,35 @@
         <v>80</v>
       </c>
       <c r="C52" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D52" t="s">
-        <v>12</v>
-      </c>
-      <c r="E52">
-        <v>40</v>
-      </c>
-      <c r="F52" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G52" s="2">
+        <v>11</v>
+      </c>
+      <c r="E52" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52">
+        <v>40</v>
+      </c>
+      <c r="G52" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H52" s="2">
         <v>1</v>
       </c>
-      <c r="H52" s="2">
+      <c r="I52" s="2">
         <v>1.8</v>
       </c>
-      <c r="I52" s="2">
+      <c r="J52" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J52">
+      <c r="K52">
         <f t="shared" si="0"/>
         <v>110.00000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>81</v>
       </c>
@@ -2919,32 +3081,35 @@
         <v>80</v>
       </c>
       <c r="C53" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D53" t="s">
-        <v>12</v>
-      </c>
-      <c r="E53">
-        <v>40</v>
-      </c>
-      <c r="F53" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G53" s="2">
+        <v>11</v>
+      </c>
+      <c r="E53" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53">
+        <v>40</v>
+      </c>
+      <c r="G53" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H53" s="2">
         <v>1</v>
       </c>
-      <c r="H53" s="2">
+      <c r="I53" s="2">
         <v>1.8</v>
       </c>
-      <c r="I53" s="2">
+      <c r="J53" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J53">
+      <c r="K53">
         <f t="shared" si="0"/>
         <v>110.00000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>82</v>
       </c>
@@ -2952,32 +3117,35 @@
         <v>83</v>
       </c>
       <c r="C54" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D54" t="s">
-        <v>12</v>
-      </c>
-      <c r="E54">
-        <v>40</v>
-      </c>
-      <c r="F54" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G54" s="2">
+        <v>11</v>
+      </c>
+      <c r="E54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54">
+        <v>40</v>
+      </c>
+      <c r="G54" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H54" s="2">
         <v>3</v>
       </c>
-      <c r="H54" s="2">
+      <c r="I54" s="2">
         <v>3.7</v>
       </c>
-      <c r="I54" s="2">
+      <c r="J54" s="2">
         <v>3.2</v>
       </c>
-      <c r="J54">
+      <c r="K54">
         <f t="shared" si="0"/>
         <v>320</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>84</v>
       </c>
@@ -2985,32 +3153,35 @@
         <v>85</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55">
-        <v>40</v>
-      </c>
-      <c r="F55" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G55" s="2">
+        <v>11</v>
+      </c>
+      <c r="E55" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55">
+        <v>40</v>
+      </c>
+      <c r="G55" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H55" s="2">
         <v>1.4</v>
       </c>
-      <c r="H55" s="2">
+      <c r="I55" s="2">
         <v>1.6</v>
       </c>
-      <c r="I55" s="2">
+      <c r="J55" s="2">
         <v>1.5</v>
       </c>
-      <c r="J55">
+      <c r="K55">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>86</v>
       </c>
@@ -3018,32 +3189,35 @@
         <v>85</v>
       </c>
       <c r="C56" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D56" t="s">
-        <v>12</v>
-      </c>
-      <c r="E56">
-        <v>40</v>
-      </c>
-      <c r="F56" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G56" s="2">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56">
+        <v>40</v>
+      </c>
+      <c r="G56" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H56" s="2">
         <v>1.5</v>
       </c>
-      <c r="H56" s="2">
+      <c r="I56" s="2">
         <v>1.7</v>
       </c>
-      <c r="I56" s="2">
+      <c r="J56" s="2">
         <v>1.6</v>
       </c>
-      <c r="J56">
+      <c r="K56">
         <f t="shared" si="0"/>
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>87</v>
       </c>
@@ -3051,32 +3225,35 @@
         <v>88</v>
       </c>
       <c r="C57" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D57" t="s">
-        <v>12</v>
-      </c>
-      <c r="E57">
-        <v>40</v>
-      </c>
-      <c r="F57" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G57" s="2">
+        <v>11</v>
+      </c>
+      <c r="E57" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57">
+        <v>40</v>
+      </c>
+      <c r="G57" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H57" s="2">
         <v>1.2</v>
       </c>
-      <c r="H57" s="2">
+      <c r="I57" s="2">
         <v>2</v>
       </c>
-      <c r="I57" s="2">
+      <c r="J57" s="2">
         <v>1.3</v>
       </c>
-      <c r="J57">
+      <c r="K57">
         <f t="shared" si="0"/>
         <v>130</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>89</v>
       </c>
@@ -3084,32 +3261,35 @@
         <v>88</v>
       </c>
       <c r="C58" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D58" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58">
-        <v>40</v>
-      </c>
-      <c r="F58" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G58" s="2">
+        <v>11</v>
+      </c>
+      <c r="E58" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58">
+        <v>40</v>
+      </c>
+      <c r="G58" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H58" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H58" s="2">
+      <c r="I58" s="2">
         <v>1.6</v>
       </c>
-      <c r="I58" s="2">
+      <c r="J58" s="2">
         <v>1.2</v>
       </c>
-      <c r="J58">
+      <c r="K58">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>90</v>
       </c>
@@ -3117,32 +3297,35 @@
         <v>91</v>
       </c>
       <c r="C59" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D59" t="s">
-        <v>12</v>
-      </c>
-      <c r="E59">
-        <v>40</v>
-      </c>
-      <c r="F59" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G59" s="2">
+        <v>11</v>
+      </c>
+      <c r="E59" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59">
+        <v>40</v>
+      </c>
+      <c r="G59" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H59" s="2">
         <v>1.7</v>
       </c>
-      <c r="H59" s="2">
+      <c r="I59" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="I59" s="2">
+      <c r="J59" s="2">
         <v>1.9</v>
       </c>
-      <c r="J59">
+      <c r="K59">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>92</v>
       </c>
@@ -3150,32 +3333,35 @@
         <v>91</v>
       </c>
       <c r="C60" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D60" t="s">
-        <v>12</v>
-      </c>
-      <c r="E60">
-        <v>40</v>
-      </c>
-      <c r="F60" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G60" s="2">
+        <v>11</v>
+      </c>
+      <c r="E60" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60">
+        <v>40</v>
+      </c>
+      <c r="G60" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H60" s="2">
         <v>1.5</v>
       </c>
-      <c r="H60" s="2">
+      <c r="I60" s="2">
         <v>1.9</v>
       </c>
-      <c r="I60" s="2">
+      <c r="J60" s="2">
         <v>1.7</v>
       </c>
-      <c r="J60">
+      <c r="K60">
         <f t="shared" si="0"/>
         <v>170</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>93</v>
       </c>
@@ -3183,32 +3369,35 @@
         <v>94</v>
       </c>
       <c r="C61" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D61" t="s">
-        <v>12</v>
-      </c>
-      <c r="E61">
-        <v>40</v>
-      </c>
-      <c r="F61" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G61" s="2">
+        <v>11</v>
+      </c>
+      <c r="E61" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61">
+        <v>40</v>
+      </c>
+      <c r="G61" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H61" s="2">
         <v>1.3</v>
       </c>
-      <c r="H61" s="2">
+      <c r="I61" s="2">
         <v>1.6</v>
       </c>
-      <c r="I61" s="2">
+      <c r="J61" s="2">
         <v>1.5</v>
       </c>
-      <c r="J61">
+      <c r="K61">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>95</v>
       </c>
@@ -3216,32 +3405,35 @@
         <v>96</v>
       </c>
       <c r="C62" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D62" t="s">
-        <v>12</v>
-      </c>
-      <c r="E62">
-        <v>40</v>
-      </c>
-      <c r="F62" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G62" s="2">
+        <v>11</v>
+      </c>
+      <c r="E62" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62">
+        <v>40</v>
+      </c>
+      <c r="G62" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H62" s="2">
         <v>1.5</v>
       </c>
-      <c r="H62" s="2">
+      <c r="I62" s="2">
         <v>2.1</v>
       </c>
-      <c r="I62" s="2">
+      <c r="J62" s="2">
         <v>1.7</v>
       </c>
-      <c r="J62">
+      <c r="K62">
         <f t="shared" si="0"/>
         <v>170</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>97</v>
       </c>
@@ -3249,32 +3441,35 @@
         <v>96</v>
       </c>
       <c r="C63" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D63" t="s">
-        <v>12</v>
-      </c>
-      <c r="E63">
-        <v>40</v>
-      </c>
-      <c r="F63" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G63" s="2">
+        <v>11</v>
+      </c>
+      <c r="E63" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63">
+        <v>40</v>
+      </c>
+      <c r="G63" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H63" s="2">
         <v>1.6</v>
       </c>
-      <c r="H63" s="2">
+      <c r="I63" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="I63" s="2">
+      <c r="J63" s="2">
         <v>1.7</v>
       </c>
-      <c r="J63">
+      <c r="K63">
         <f t="shared" si="0"/>
         <v>170</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>98</v>
       </c>
@@ -3282,32 +3477,35 @@
         <v>96</v>
       </c>
       <c r="C64" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D64" t="s">
-        <v>12</v>
-      </c>
-      <c r="E64">
-        <v>40</v>
-      </c>
-      <c r="F64" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G64" s="2">
+        <v>11</v>
+      </c>
+      <c r="E64" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64">
+        <v>40</v>
+      </c>
+      <c r="G64" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H64" s="2">
         <v>1.6</v>
       </c>
-      <c r="H64" s="2">
+      <c r="I64" s="2">
         <v>2.1</v>
       </c>
-      <c r="I64" s="2">
+      <c r="J64" s="2">
         <v>1.8</v>
       </c>
-      <c r="J64">
+      <c r="K64">
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>99</v>
       </c>
@@ -3315,27 +3513,30 @@
         <v>96</v>
       </c>
       <c r="C65" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D65" t="s">
-        <v>12</v>
-      </c>
-      <c r="E65">
-        <v>40</v>
-      </c>
-      <c r="F65" s="1">
-        <v>45931</v>
-      </c>
-      <c r="G65" s="2">
+        <v>11</v>
+      </c>
+      <c r="E65" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65">
+        <v>40</v>
+      </c>
+      <c r="G65" s="1">
+        <v>45931</v>
+      </c>
+      <c r="H65" s="2">
         <v>1</v>
       </c>
-      <c r="H65" s="2">
+      <c r="I65" s="2">
         <v>1.3</v>
       </c>
-      <c r="I65" s="2">
+      <c r="J65" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J65">
+      <c r="K65">
         <f t="shared" si="0"/>
         <v>110.00000000000001</v>
       </c>

</xml_diff>

<commit_message>
small changes on abastecedor 2
</commit_message>
<xml_diff>
--- a/Datasets/Abastecedores_2025-10-01_2025-10-01.xlsx
+++ b/Datasets/Abastecedores_2025-10-01_2025-10-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofia\Documents\Data_Analytics_Ironhack\Projects\ironhack_final_project\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{14EEFA7F-F1F7-4720-A2B5-BA2ED84F3AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{EAB616D0-B608-464F-97D0-B64E5AB09B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{2A4A056C-2E7C-40E0-AC2B-3807CB21F695}"/>
   </bookViews>
@@ -325,10 +325,10 @@
     <t>€/100kg</t>
   </si>
   <si>
-    <t>Categoria</t>
-  </si>
-  <si>
     <t>Frutos</t>
+  </si>
+  <si>
+    <t>categoria</t>
   </si>
 </sst>
 </file>
@@ -1194,7 +1194,7 @@
   <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1210,7 +1210,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1245,7 +1245,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -1281,7 +1281,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -1317,7 +1317,7 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -1353,7 +1353,7 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -1389,7 +1389,7 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -1425,7 +1425,7 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -1461,7 +1461,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -1497,7 +1497,7 @@
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1533,7 +1533,7 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -1569,7 +1569,7 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -1605,7 +1605,7 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -1641,7 +1641,7 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -1677,7 +1677,7 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -1713,7 +1713,7 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -1749,7 +1749,7 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -1785,7 +1785,7 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
@@ -1821,7 +1821,7 @@
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
@@ -1857,7 +1857,7 @@
         <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -1893,7 +1893,7 @@
         <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -1929,7 +1929,7 @@
         <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -1965,7 +1965,7 @@
         <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -2001,7 +2001,7 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
@@ -2037,7 +2037,7 @@
         <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -2073,7 +2073,7 @@
         <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
@@ -2109,7 +2109,7 @@
         <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -2145,7 +2145,7 @@
         <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -2181,7 +2181,7 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -2217,7 +2217,7 @@
         <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -2253,7 +2253,7 @@
         <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
@@ -2289,7 +2289,7 @@
         <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -2325,7 +2325,7 @@
         <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -2361,7 +2361,7 @@
         <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -2397,7 +2397,7 @@
         <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
@@ -2433,7 +2433,7 @@
         <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
@@ -2469,7 +2469,7 @@
         <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
@@ -2505,7 +2505,7 @@
         <v>52</v>
       </c>
       <c r="C37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
@@ -2541,7 +2541,7 @@
         <v>52</v>
       </c>
       <c r="C38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D38" t="s">
         <v>11</v>
@@ -2577,7 +2577,7 @@
         <v>52</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -2613,7 +2613,7 @@
         <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D40" t="s">
         <v>11</v>
@@ -2649,7 +2649,7 @@
         <v>64</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -2685,7 +2685,7 @@
         <v>64</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
@@ -2721,7 +2721,7 @@
         <v>68</v>
       </c>
       <c r="C43" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -2757,7 +2757,7 @@
         <v>68</v>
       </c>
       <c r="C44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -2793,7 +2793,7 @@
         <v>68</v>
       </c>
       <c r="C45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
@@ -2829,7 +2829,7 @@
         <v>68</v>
       </c>
       <c r="C46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
@@ -2865,7 +2865,7 @@
         <v>73</v>
       </c>
       <c r="C47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -2901,7 +2901,7 @@
         <v>73</v>
       </c>
       <c r="C48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D48" t="s">
         <v>11</v>
@@ -2937,7 +2937,7 @@
         <v>73</v>
       </c>
       <c r="C49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
@@ -2973,7 +2973,7 @@
         <v>73</v>
       </c>
       <c r="C50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D50" t="s">
         <v>11</v>
@@ -3009,7 +3009,7 @@
         <v>78</v>
       </c>
       <c r="C51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
@@ -3045,7 +3045,7 @@
         <v>80</v>
       </c>
       <c r="C52" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D52" t="s">
         <v>11</v>
@@ -3081,7 +3081,7 @@
         <v>80</v>
       </c>
       <c r="C53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
@@ -3117,7 +3117,7 @@
         <v>83</v>
       </c>
       <c r="C54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D54" t="s">
         <v>11</v>
@@ -3153,7 +3153,7 @@
         <v>85</v>
       </c>
       <c r="C55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
@@ -3189,7 +3189,7 @@
         <v>85</v>
       </c>
       <c r="C56" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D56" t="s">
         <v>11</v>
@@ -3225,7 +3225,7 @@
         <v>88</v>
       </c>
       <c r="C57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D57" t="s">
         <v>11</v>
@@ -3261,7 +3261,7 @@
         <v>88</v>
       </c>
       <c r="C58" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
@@ -3297,7 +3297,7 @@
         <v>91</v>
       </c>
       <c r="C59" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D59" t="s">
         <v>11</v>
@@ -3333,7 +3333,7 @@
         <v>91</v>
       </c>
       <c r="C60" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D60" t="s">
         <v>11</v>
@@ -3369,7 +3369,7 @@
         <v>94</v>
       </c>
       <c r="C61" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D61" t="s">
         <v>11</v>
@@ -3405,7 +3405,7 @@
         <v>96</v>
       </c>
       <c r="C62" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D62" t="s">
         <v>11</v>
@@ -3441,7 +3441,7 @@
         <v>96</v>
       </c>
       <c r="C63" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D63" t="s">
         <v>11</v>
@@ -3477,7 +3477,7 @@
         <v>96</v>
       </c>
       <c r="C64" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D64" t="s">
         <v>11</v>
@@ -3513,7 +3513,7 @@
         <v>96</v>
       </c>
       <c r="C65" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D65" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
small changes abastecedor 4
</commit_message>
<xml_diff>
--- a/Datasets/Abastecedores_2025-10-01_2025-10-01.xlsx
+++ b/Datasets/Abastecedores_2025-10-01_2025-10-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofia\Documents\Data_Analytics_Ironhack\Projects\ironhack_final_project\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{EAB616D0-B608-464F-97D0-B64E5AB09B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{EBDC88C7-55FB-4FD5-8553-E5EFA0319D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{2A4A056C-2E7C-40E0-AC2B-3807CB21F695}"/>
   </bookViews>
@@ -322,13 +322,13 @@
     <t>Uva*Vitória*II*Caixa*Nacional*EUR/kg</t>
   </si>
   <si>
-    <t>€/100kg</t>
-  </si>
-  <si>
     <t>Frutos</t>
   </si>
   <si>
     <t>categoria</t>
+  </si>
+  <si>
+    <t>Preco</t>
   </si>
 </sst>
 </file>
@@ -1194,7 +1194,7 @@
   <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1210,7 +1210,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1234,7 +1234,7 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
@@ -1245,7 +1245,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -1281,7 +1281,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -1317,7 +1317,7 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -1353,7 +1353,7 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -1389,7 +1389,7 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -1425,7 +1425,7 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -1461,7 +1461,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -1497,7 +1497,7 @@
         <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1533,7 +1533,7 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -1569,7 +1569,7 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -1605,7 +1605,7 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -1641,7 +1641,7 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -1677,7 +1677,7 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -1713,7 +1713,7 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -1749,7 +1749,7 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -1785,7 +1785,7 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
@@ -1821,7 +1821,7 @@
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
@@ -1857,7 +1857,7 @@
         <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -1893,7 +1893,7 @@
         <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -1929,7 +1929,7 @@
         <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -1965,7 +1965,7 @@
         <v>40</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -2001,7 +2001,7 @@
         <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
@@ -2037,7 +2037,7 @@
         <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -2073,7 +2073,7 @@
         <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
@@ -2109,7 +2109,7 @@
         <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -2145,7 +2145,7 @@
         <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -2181,7 +2181,7 @@
         <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -2217,7 +2217,7 @@
         <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D29" t="s">
         <v>11</v>
@@ -2253,7 +2253,7 @@
         <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
@@ -2289,7 +2289,7 @@
         <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -2325,7 +2325,7 @@
         <v>52</v>
       </c>
       <c r="C32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D32" t="s">
         <v>11</v>
@@ -2361,7 +2361,7 @@
         <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -2397,7 +2397,7 @@
         <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
@@ -2433,7 +2433,7 @@
         <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D35" t="s">
         <v>11</v>
@@ -2469,7 +2469,7 @@
         <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D36" t="s">
         <v>11</v>
@@ -2505,7 +2505,7 @@
         <v>52</v>
       </c>
       <c r="C37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
@@ -2541,7 +2541,7 @@
         <v>52</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D38" t="s">
         <v>11</v>
@@ -2577,7 +2577,7 @@
         <v>52</v>
       </c>
       <c r="C39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -2613,7 +2613,7 @@
         <v>64</v>
       </c>
       <c r="C40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D40" t="s">
         <v>11</v>
@@ -2649,7 +2649,7 @@
         <v>64</v>
       </c>
       <c r="C41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -2685,7 +2685,7 @@
         <v>64</v>
       </c>
       <c r="C42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
@@ -2721,7 +2721,7 @@
         <v>68</v>
       </c>
       <c r="C43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -2757,7 +2757,7 @@
         <v>68</v>
       </c>
       <c r="C44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D44" t="s">
         <v>11</v>
@@ -2793,7 +2793,7 @@
         <v>68</v>
       </c>
       <c r="C45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
@@ -2829,7 +2829,7 @@
         <v>68</v>
       </c>
       <c r="C46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D46" t="s">
         <v>11</v>
@@ -2865,7 +2865,7 @@
         <v>73</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -2901,7 +2901,7 @@
         <v>73</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D48" t="s">
         <v>11</v>
@@ -2937,7 +2937,7 @@
         <v>73</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D49" t="s">
         <v>11</v>
@@ -2973,7 +2973,7 @@
         <v>73</v>
       </c>
       <c r="C50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D50" t="s">
         <v>11</v>
@@ -3009,7 +3009,7 @@
         <v>78</v>
       </c>
       <c r="C51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D51" t="s">
         <v>11</v>
@@ -3045,7 +3045,7 @@
         <v>80</v>
       </c>
       <c r="C52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D52" t="s">
         <v>11</v>
@@ -3081,7 +3081,7 @@
         <v>80</v>
       </c>
       <c r="C53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
@@ -3117,7 +3117,7 @@
         <v>83</v>
       </c>
       <c r="C54" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D54" t="s">
         <v>11</v>
@@ -3153,7 +3153,7 @@
         <v>85</v>
       </c>
       <c r="C55" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
@@ -3189,7 +3189,7 @@
         <v>85</v>
       </c>
       <c r="C56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D56" t="s">
         <v>11</v>
@@ -3225,7 +3225,7 @@
         <v>88</v>
       </c>
       <c r="C57" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D57" t="s">
         <v>11</v>
@@ -3261,7 +3261,7 @@
         <v>88</v>
       </c>
       <c r="C58" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D58" t="s">
         <v>11</v>
@@ -3297,7 +3297,7 @@
         <v>91</v>
       </c>
       <c r="C59" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D59" t="s">
         <v>11</v>
@@ -3333,7 +3333,7 @@
         <v>91</v>
       </c>
       <c r="C60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D60" t="s">
         <v>11</v>
@@ -3369,7 +3369,7 @@
         <v>94</v>
       </c>
       <c r="C61" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D61" t="s">
         <v>11</v>
@@ -3405,7 +3405,7 @@
         <v>96</v>
       </c>
       <c r="C62" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D62" t="s">
         <v>11</v>
@@ -3441,7 +3441,7 @@
         <v>96</v>
       </c>
       <c r="C63" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D63" t="s">
         <v>11</v>
@@ -3477,7 +3477,7 @@
         <v>96</v>
       </c>
       <c r="C64" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D64" t="s">
         <v>11</v>
@@ -3513,7 +3513,7 @@
         <v>96</v>
       </c>
       <c r="C65" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D65" t="s">
         <v>11</v>

</xml_diff>